<commit_message>
Version correcciones sin escribir
</commit_message>
<xml_diff>
--- a/Recursos/metodologia.xlsx
+++ b/Recursos/metodologia.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Causas</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Alumno</t>
   </si>
   <si>
-    <t>Dificultad para trabajar en grupo</t>
-  </si>
-  <si>
     <t>Carga inequitiva de trabjo</t>
   </si>
   <si>
@@ -111,6 +108,15 @@
   </si>
   <si>
     <t>Para esto debería cambiar la identificacion del problema</t>
+  </si>
+  <si>
+    <t>O como hacer hipotesis en usabilidad?</t>
+  </si>
+  <si>
+    <t>U otra</t>
+  </si>
+  <si>
+    <t>Percepcion de carga nota</t>
   </si>
 </sst>
 </file>
@@ -565,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F39"/>
+  <dimension ref="B1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,19 +586,19 @@
     <col min="7" max="7" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -603,24 +609,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -629,61 +635,64 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -693,41 +702,41 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
       <c r="D21" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="6"/>
       <c r="D22" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
       <c r="D23" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -739,7 +748,7 @@
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
       <c r="D25" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -749,19 +758,19 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C31" s="16"/>
       <c r="D31" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -771,38 +780,40 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="6"/>
       <c r="D34" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
+      <c r="B35" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="C35" s="6"/>
       <c r="D35" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="C36" s="6"/>
       <c r="D36" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -810,7 +821,7 @@
       <c r="C37" s="6"/>
       <c r="D37" s="13"/>
       <c r="F37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -822,6 +833,11 @@
       <c r="B39" s="9"/>
       <c r="C39" s="10"/>
       <c r="D39" s="14"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>